<commit_message>
Thêm các file âm thanh. Xóa một file demo không cần thiết (nặng). Bỏ phần xử lý chuột.
</commit_message>
<xml_diff>
--- a/ChecklistReference.xlsx
+++ b/ChecklistReference.xlsx
@@ -11,19 +11,58 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="124519"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>Nén mp3</t>
+  </si>
+  <si>
+    <t>http://www.yoyogames.com/resources?cat_id=4</t>
+  </si>
+  <si>
+    <t>The Witcher 2 Bonus Disc</t>
+  </si>
+  <si>
+    <t>Bejeweled 2</t>
+  </si>
+  <si>
+    <t>http://www.gamedev.net/topic/272386-sprites-sprites-and-more-sprites/</t>
+  </si>
+  <si>
+    <t>Các tập tin âm thanh (mp3, wav)</t>
+  </si>
+  <si>
+    <t>Các tập tin hình ảnh (jpg)</t>
+  </si>
+  <si>
+    <t>EKOS MP3Minimizer</t>
+  </si>
+  <si>
+    <t>Resource cung cấp trong môn học C4W</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -43,13 +82,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -342,12 +387,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>